<commit_message>
Adjust drop rate of frags and super rares.
</commit_message>
<xml_diff>
--- a/_Design doc - Sosiggun Soren.xlsx
+++ b/_Design doc - Sosiggun Soren.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Projects\Gamedev - SR Sosiggun Soren\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59313CB9-7247-4F12-9377-0A3399B1E545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE92B2D-67E0-4F56-B079-A293036AF3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{7310D13B-FF44-461A-9DD2-8B991C400D59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7310D13B-FF44-461A-9DD2-8B991C400D59}"/>
   </bookViews>
   <sheets>
     <sheet name="All sosigguns 2024-01-03" sheetId="1" r:id="rId1"/>
@@ -2137,9 +2137,9 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.000000%"/>
-    <numFmt numFmtId="169" formatCode="0.000%"/>
-    <numFmt numFmtId="170" formatCode="0.0E+00"/>
-    <numFmt numFmtId="171" formatCode="0.0000%"/>
+    <numFmt numFmtId="167" formatCode="0.000%"/>
+    <numFmt numFmtId="168" formatCode="0.0E+00"/>
+    <numFmt numFmtId="169" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -2411,12 +2411,12 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7394,7 +7394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5054F299-DF91-4684-8BD5-2083CF7C1A86}">
   <dimension ref="A1:U54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
@@ -10621,8 +10621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69962C0B-4472-4DA9-BA98-8FB221EC5760}">
   <dimension ref="C3:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10658,15 +10658,15 @@
         <v>630</v>
       </c>
       <c r="D4" s="37">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="E4" s="38">
         <f>1-D4</f>
-        <v>0.97</v>
+        <v>0.94</v>
       </c>
       <c r="F4" s="36">
         <f t="shared" ref="F4:F7" si="0">D4</f>
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="G4" s="35"/>
       <c r="H4" s="34"/>
@@ -10714,15 +10714,15 @@
         <v>689</v>
       </c>
       <c r="D7" s="37">
-        <v>1.2E-4</v>
+        <v>2.4000000000000001E-4</v>
       </c>
       <c r="E7" s="38">
         <f t="shared" si="1"/>
-        <v>0.99987999999999999</v>
+        <v>0.99975999999999998</v>
       </c>
       <c r="F7" s="36">
         <f t="shared" si="0"/>
-        <v>1.2E-4</v>
+        <v>2.4000000000000001E-4</v>
       </c>
       <c r="G7" s="35"/>
       <c r="H7" s="34"/>
@@ -10743,7 +10743,7 @@
       <c r="D9" s="37"/>
       <c r="E9" s="38">
         <f>E5*E4*E6*E7</f>
-        <v>0.80228771391999998</v>
+        <v>0.77738138367999987</v>
       </c>
       <c r="F9" s="35"/>
       <c r="G9" s="35"/>
@@ -10756,7 +10756,7 @@
       <c r="D10" s="37"/>
       <c r="E10" s="38">
         <f>1-E9</f>
-        <v>0.19771228608000002</v>
+        <v>0.22261861632000013</v>
       </c>
       <c r="F10" s="35"/>
       <c r="G10" s="35"/>
@@ -10783,7 +10783,7 @@
       <c r="D12" s="38"/>
       <c r="E12" s="38">
         <f>1-(E6*E7)</f>
-        <v>0.12010560000000003</v>
+        <v>0.12021119999999996</v>
       </c>
       <c r="G12" s="38"/>
     </row>
@@ -10794,7 +10794,7 @@
       <c r="D13" s="38"/>
       <c r="E13" s="38">
         <f>1-(E5*E4)</f>
-        <v>8.8200000000000056E-2</v>
+        <v>0.11640000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Economy changes following loot drop boost
</commit_message>
<xml_diff>
--- a/_Design doc - Sosiggun Soren.xlsx
+++ b/_Design doc - Sosiggun Soren.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Projects\Gamedev - SR Sosiggun Soren\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE92B2D-67E0-4F56-B079-A293036AF3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C3A850-5FD3-4F46-894C-020ECAE13B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7310D13B-FF44-461A-9DD2-8B991C400D59}"/>
   </bookViews>
@@ -10622,7 +10622,7 @@
   <dimension ref="C3:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10658,15 +10658,15 @@
         <v>630</v>
       </c>
       <c r="D4" s="37">
-        <v>0.06</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E4" s="38">
         <f>1-D4</f>
-        <v>0.94</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="F4" s="36">
         <f t="shared" ref="F4:F7" si="0">D4</f>
-        <v>0.06</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G4" s="35"/>
       <c r="H4" s="34"/>
@@ -10677,15 +10677,15 @@
         <v>691</v>
       </c>
       <c r="D5" s="37">
-        <v>0.06</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E5" s="38">
         <f>1-D5</f>
-        <v>0.94</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="F5" s="36">
         <f>D5</f>
-        <v>0.06</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G5" s="35"/>
       <c r="H5" s="34"/>
@@ -10708,6 +10708,7 @@
       </c>
       <c r="G6" s="35"/>
       <c r="H6" s="34"/>
+      <c r="I6" s="35"/>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C7" s="19" t="s">
@@ -10726,6 +10727,7 @@
       </c>
       <c r="G7" s="35"/>
       <c r="H7" s="34"/>
+      <c r="I7" s="35"/>
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C8" s="19"/>
@@ -10734,6 +10736,7 @@
       <c r="F8" s="35"/>
       <c r="G8" s="35"/>
       <c r="H8" s="34"/>
+      <c r="I8" s="35"/>
       <c r="K8" s="39"/>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.25">
@@ -10743,11 +10746,12 @@
       <c r="D9" s="37"/>
       <c r="E9" s="38">
         <f>E5*E4*E6*E7</f>
-        <v>0.77738138367999987</v>
+        <v>0.80238938031999996</v>
       </c>
       <c r="F9" s="35"/>
       <c r="G9" s="35"/>
       <c r="H9" s="34"/>
+      <c r="I9" s="35"/>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C10" s="19" t="s">
@@ -10756,11 +10760,12 @@
       <c r="D10" s="37"/>
       <c r="E10" s="38">
         <f>1-E9</f>
-        <v>0.22261861632000013</v>
+        <v>0.19761061968000004</v>
       </c>
       <c r="F10" s="35"/>
       <c r="G10" s="35"/>
       <c r="H10" s="39"/>
+      <c r="I10" s="35"/>
       <c r="K10" s="40"/>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.25">
@@ -10770,11 +10775,12 @@
       <c r="D11" s="37"/>
       <c r="E11" s="38">
         <f>1-(E5)</f>
-        <v>6.0000000000000053E-2</v>
+        <v>4.500000000000004E-2</v>
       </c>
       <c r="F11" s="35"/>
       <c r="G11" s="35"/>
       <c r="H11" s="34"/>
+      <c r="I11" s="35"/>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C12" s="19" t="s">
@@ -10786,6 +10792,7 @@
         <v>0.12021119999999996</v>
       </c>
       <c r="G12" s="38"/>
+      <c r="I12" s="35"/>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C13" s="19" t="s">
@@ -10794,8 +10801,9 @@
       <c r="D13" s="38"/>
       <c r="E13" s="38">
         <f>1-(E5*E4)</f>
-        <v>0.11640000000000006</v>
-      </c>
+        <v>8.7975000000000025E-2</v>
+      </c>
+      <c r="I13" s="35"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M26:N31">

</xml_diff>